<commit_message>
Updating the WBS excel sheet slightly.
The gantt schedule title cell was too small and didnt stretch the full 3 weeks
</commit_message>
<xml_diff>
--- a/Root 9 WBS.xlsx
+++ b/Root 9 WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2eba328ab996dff9/Work/Smartsheet_Publishing/Templates for Update/Gantt Chart Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E083C0D4-422D-4750-88E0-4CBEC2AA15D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E726FC4-36F6-4AE5-922E-E1ACD9C7D182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38460" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -832,30 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </left>
@@ -910,6 +886,15 @@
       <bottom style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1091,10 +1076,10 @@
     <xf numFmtId="16" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,10 +1091,10 @@
     <xf numFmtId="16" fontId="3" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1340,8 +1325,8 @@
   <dimension ref="B1:AC34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5:AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1405,22 +1390,29 @@
     </row>
     <row r="5" spans="2:29" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="B5" s="2"/>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="3" t="s">
@@ -1444,33 +1436,33 @@
       <c r="H6" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="66">
         <v>45222</v>
       </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="63"/>
-      <c r="P6" s="66">
+      <c r="P6" s="64">
         <v>45229</v>
       </c>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="69">
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="67">
         <v>45236</v>
       </c>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="70"/>
-      <c r="AA6" s="70"/>
-      <c r="AB6" s="70"/>
-      <c r="AC6" s="70"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="68"/>
+      <c r="Z6" s="68"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
     </row>
     <row r="7" spans="2:29" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="6" t="s">
@@ -2645,7 +2637,7 @@
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="P6:V6"/>
     <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="I5:V5"/>
+    <mergeCell ref="I5:AC5"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:H34">
     <cfRule type="dataBar" priority="8">

</xml_diff>